<commit_message>
v5 - sept 2023
</commit_message>
<xml_diff>
--- a/data/raw/superkneedata notes.xlsx
+++ b/data/raw/superkneedata notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickgirdwood/r/superkdataclean/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8F605A-FF68-DD44-9F83-47C95A52B5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF12DEA-D980-DB45-9CE3-4DA8AEE02B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="500" windowWidth="26840" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="1326">
   <si>
     <t>newname</t>
   </si>
@@ -3908,6 +3908,96 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>surgery_information_timestamp</t>
+  </si>
+  <si>
+    <t>sx_name</t>
+  </si>
+  <si>
+    <t>sx_hospital</t>
+  </si>
+  <si>
+    <t>sx_primary</t>
+  </si>
+  <si>
+    <t>sx_side</t>
+  </si>
+  <si>
+    <t>sx_graft</t>
+  </si>
+  <si>
+    <t>sx_graft_other</t>
+  </si>
+  <si>
+    <t>sx_graftside</t>
+  </si>
+  <si>
+    <t>sx_meniscus</t>
+  </si>
+  <si>
+    <t>sx_meniscus_other</t>
+  </si>
+  <si>
+    <t>sx_meniscus_lat</t>
+  </si>
+  <si>
+    <t>sx_meniscus_other_lat</t>
+  </si>
+  <si>
+    <t>sx_patellacartilage</t>
+  </si>
+  <si>
+    <t>sx_trochleacartilage</t>
+  </si>
+  <si>
+    <t>sx_tibialcartilage</t>
+  </si>
+  <si>
+    <t>sx_tibiallatcartilage</t>
+  </si>
+  <si>
+    <t>sx_femoralcartilage</t>
+  </si>
+  <si>
+    <t>sx_femorallatcartilage</t>
+  </si>
+  <si>
+    <t>sx_cartilage_int</t>
+  </si>
+  <si>
+    <t>sx_cartilage_int_other</t>
+  </si>
+  <si>
+    <t>sx_other</t>
+  </si>
+  <si>
+    <t>sx_extradetails</t>
+  </si>
+  <si>
+    <t>surgery_information_complete</t>
+  </si>
+  <si>
+    <t>sx_meniscus_lat_other</t>
+  </si>
+  <si>
+    <t>sx_meniscus_med</t>
+  </si>
+  <si>
+    <t>sx_meniscus_med_other</t>
+  </si>
+  <si>
+    <t>sx_tibialcartilage_med</t>
+  </si>
+  <si>
+    <t>sx_tibialcartilage_lat</t>
+  </si>
+  <si>
+    <t>sx_femoralcartilage_med</t>
+  </si>
+  <si>
+    <t>sx_femoralcartilage_lat</t>
   </si>
 </sst>
 </file>
@@ -4748,10 +4838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E954"/>
+  <dimension ref="A1:E977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A937" workbookViewId="0">
-      <selection activeCell="B956" sqref="B956"/>
+    <sheetView tabSelected="1" topLeftCell="A928" workbookViewId="0">
+      <selection activeCell="E976" sqref="E976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13445,9 +13535,6 @@
       <c r="B942" t="s">
         <v>1232</v>
       </c>
-      <c r="C942" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A943" t="s">
@@ -13543,6 +13630,190 @@
       </c>
       <c r="B954" t="s">
         <v>1295</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A955" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A956" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A957" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A958" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A959" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A960" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A961" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A962" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A963" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A964" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A965" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A966" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A967" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A968" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A969" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B969" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A970" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A971" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A972" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A973" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A974" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B974" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A975" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A976" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B976" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A977" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B977" t="s">
+        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>